<commit_message>
19.08.2024 - Możliwe jest wprowadzenie wszystkich danych stałych. Rozpoczynam pracę nad przeliczaniem nieobecności
</commit_message>
<xml_diff>
--- a/bledy/bledy.xlsx
+++ b/bledy/bledy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjektyPython\place_v1\bledy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjektyPython\place_v2\bledy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF38E88-B9F1-473B-848A-504D267EB851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E92FFE-7573-4857-A791-CA4B841FE03C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1080" windowWidth="25350" windowHeight="11490" xr2:uid="{9A003B67-5788-410F-A333-A87AA62D4358}"/>
+    <workbookView xWindow="5025" yWindow="1740" windowWidth="22575" windowHeight="11490" xr2:uid="{9A003B67-5788-410F-A333-A87AA62D4358}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -36,52 +36,211 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>lp</t>
   </si>
   <si>
-    <t>nr</t>
-  </si>
-  <si>
-    <t>kto</t>
-  </si>
-  <si>
-    <t>ile</t>
-  </si>
-  <si>
-    <t>aa</t>
-  </si>
-  <si>
-    <t>ss</t>
-  </si>
-  <si>
-    <t>dd</t>
-  </si>
-  <si>
-    <t>ff</t>
-  </si>
-  <si>
-    <t>gg</t>
-  </si>
-  <si>
-    <t>hh</t>
-  </si>
-  <si>
-    <t>jj</t>
-  </si>
-  <si>
-    <t>kk</t>
-  </si>
-  <si>
-    <t>ll</t>
+    <t>nr pracownika</t>
+  </si>
+  <si>
+    <t>IMIĘ i NAZWISKO</t>
+  </si>
+  <si>
+    <t>Suma z błędów</t>
+  </si>
+  <si>
+    <t>Orlicka Maria</t>
+  </si>
+  <si>
+    <t>Tynna Beata</t>
+  </si>
+  <si>
+    <t>KAŹMIERCZAK SYLWIA</t>
+  </si>
+  <si>
+    <t>Rogozinska Katarzyna</t>
+  </si>
+  <si>
+    <t>Kraska Boguslawa</t>
+  </si>
+  <si>
+    <t>Zawierucha_ Ilona</t>
+  </si>
+  <si>
+    <t>SIMIŃSKA MAŁGORZATA</t>
+  </si>
+  <si>
+    <t>Czaplicka Anna</t>
+  </si>
+  <si>
+    <t>Urban Dorota</t>
+  </si>
+  <si>
+    <t>SZYNAL ELŻBIETA</t>
+  </si>
+  <si>
+    <t>SAS Aneta</t>
+  </si>
+  <si>
+    <t>SZYNAL ANNA</t>
+  </si>
+  <si>
+    <t>GÓRALCZYK ANNA</t>
+  </si>
+  <si>
+    <t>SIERPIEJKO KATARZYNA</t>
+  </si>
+  <si>
+    <t>HALMAN ANNA</t>
+  </si>
+  <si>
+    <t>Maksymiuk Andrzej</t>
+  </si>
+  <si>
+    <t>Gancarz Beata</t>
+  </si>
+  <si>
+    <t>Czajka Iwona</t>
+  </si>
+  <si>
+    <t>Jałowiecka Melania</t>
+  </si>
+  <si>
+    <t>Rowicka Dorota</t>
+  </si>
+  <si>
+    <t>Szczepańska Małgorzata</t>
+  </si>
+  <si>
+    <t>LUKAS LUCYNA</t>
+  </si>
+  <si>
+    <t>Gil Anna</t>
+  </si>
+  <si>
+    <t>Gadek Agnieszka</t>
+  </si>
+  <si>
+    <t>KUZIO ADRIAN</t>
+  </si>
+  <si>
+    <t>Nowakowska Edyta</t>
+  </si>
+  <si>
+    <t>Żych Paulina</t>
+  </si>
+  <si>
+    <t>Skiba Aneta</t>
+  </si>
+  <si>
+    <t>Kasprzycka Renata</t>
+  </si>
+  <si>
+    <t>Walczak Bartosz</t>
+  </si>
+  <si>
+    <t>Krawniak Zofia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JESCHKE KAROLINA </t>
+  </si>
+  <si>
+    <t>Bieniek Elżbieta</t>
+  </si>
+  <si>
+    <t>Giwojno Ilona</t>
+  </si>
+  <si>
+    <t>Matysiak Anna</t>
+  </si>
+  <si>
+    <t>Osowski Sebastian</t>
+  </si>
+  <si>
+    <t>Sobotot Adrian</t>
+  </si>
+  <si>
+    <t>Tober Krzysztof</t>
+  </si>
+  <si>
+    <t>Michalak Jakub</t>
+  </si>
+  <si>
+    <t>MALLEK KAMIL</t>
+  </si>
+  <si>
+    <t>Stachnik_ Aleksandra</t>
+  </si>
+  <si>
+    <t>Antczak Dariusz</t>
+  </si>
+  <si>
+    <t>Swarcewicz_ Anna</t>
+  </si>
+  <si>
+    <t>Taudul Natalia</t>
+  </si>
+  <si>
+    <t>Pawulski Piotr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUJNOWSKA VIOLETTA </t>
+  </si>
+  <si>
+    <t>Bulicki Zbigniew</t>
+  </si>
+  <si>
+    <t>Wójcicka Iwona</t>
+  </si>
+  <si>
+    <t>Smołucha Aneta</t>
+  </si>
+  <si>
+    <t>Wojtkowska Anna</t>
+  </si>
+  <si>
+    <t>Hrybowicz Wojciech</t>
+  </si>
+  <si>
+    <t>PIOTROWSKI  GRZEGORZ</t>
+  </si>
+  <si>
+    <t>Siana Charisa</t>
+  </si>
+  <si>
+    <t>FIKRI MUHAMMAD RIZAL</t>
+  </si>
+  <si>
+    <t>Dura Salas</t>
+  </si>
+  <si>
+    <t>DOJOHARUDIN</t>
+  </si>
+  <si>
+    <t>Afrianto Heri</t>
+  </si>
+  <si>
+    <t>Nebab Ginia</t>
+  </si>
+  <si>
+    <t>Maybenig Cendy</t>
+  </si>
+  <si>
+    <t>MENDEZ GALINDO ANNA MARIA</t>
+  </si>
+  <si>
+    <t>Botina Karen Tatiana</t>
+  </si>
+  <si>
+    <t>ORTEGA CARO JOEL DAVID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,13 +249,34 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -108,14 +288,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny 2" xfId="1" xr:uid="{C916F75C-91C5-4B75-9C8B-AD72B44F931A}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -447,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E83883C-EB99-482A-92BF-3645C56F7AE9}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="A2" sqref="A2:A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,13 +645,13 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -473,55 +659,55 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="2">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2">
-        <v>5</v>
+      <c r="D2" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" s="2">
+        <v>29</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3">
-        <v>2</v>
+      <c r="D3" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" s="2">
+        <v>76</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4">
-        <v>3</v>
+      <c r="D4" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B5" s="2">
+        <v>93</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>1</v>
       </c>
     </row>
@@ -529,13 +715,13 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6">
+      <c r="B6" s="2">
+        <v>117</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="2">
         <v>1</v>
       </c>
     </row>
@@ -543,13 +729,13 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7">
+      <c r="B7" s="2">
+        <v>253</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="2">
         <v>2</v>
       </c>
     </row>
@@ -557,13 +743,13 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>29</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8">
+      <c r="B8" s="2">
+        <v>263</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="2">
         <v>1</v>
       </c>
     </row>
@@ -571,27 +757,769 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>57</v>
-      </c>
-      <c r="C9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9">
-        <v>4</v>
+      <c r="B9" s="2">
+        <v>283</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
+        <v>428</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1354</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1501</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1515</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1522</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1702</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1765</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1789</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1799</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1814</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1825</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1877</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1883</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1907</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1954</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2">
+        <v>1982</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2">
+        <v>2009</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2">
+        <v>2037</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2">
+        <v>2104</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2">
+        <v>2118</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2">
+        <v>2132</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2">
+        <v>2136</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2">
+        <v>2139</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2">
+        <v>2150</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D34" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" s="2">
+        <v>2262</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" s="2">
+        <v>2293</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" s="2">
+        <v>2612</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" s="2">
+        <v>2697</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D38" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" s="2">
+        <v>2705</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D39" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" s="2">
+        <v>2706</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" s="2">
+        <v>2726</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D41" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" s="2">
+        <v>2866</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D42" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" s="2">
+        <v>2882</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D43" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" s="2">
+        <v>2885</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D44" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" s="2">
+        <v>2922</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D45" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" s="2">
+        <v>2926</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D46" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" s="2">
+        <v>2960</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D47" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" s="2">
+        <v>3005</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D48" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" s="2">
+        <v>3054</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D49" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" s="2">
+        <v>3165</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D50" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" s="2">
+        <v>3179</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D51" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" s="2">
+        <v>3185</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D52" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" s="2">
+        <v>3243</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D53" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" s="2">
+        <v>6009</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D54" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" s="2">
+        <v>6025</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D55" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" s="2">
+        <v>6034</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D56" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" s="2">
+        <v>6058</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D57" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" s="2">
+        <v>6084</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10">
+      <c r="D58" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" s="2">
+        <v>6094</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D59" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" s="2">
+        <v>6102</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D60" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" s="2">
+        <v>6105</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D61" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" s="2">
+        <v>6165</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D62" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" s="2">
+        <v>6172</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D63" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
07.10.2024 - Zmiana sposobu zliczania premii pracowników. Problem nie jest rozwiązany. Zapytanie błędnie liczy kwoty
</commit_message>
<xml_diff>
--- a/bledy/bledy.xlsx
+++ b/bledy/bledy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjektyPython\place_v2\bledy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mirek\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E92FFE-7573-4857-A791-CA4B841FE03C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D27779F-67D5-4710-9918-BFD1776FF4E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5025" yWindow="1740" windowWidth="22575" windowHeight="11490" xr2:uid="{9A003B67-5788-410F-A333-A87AA62D4358}"/>
+    <workbookView xWindow="12165" yWindow="915" windowWidth="23475" windowHeight="11760" xr2:uid="{9A003B67-5788-410F-A333-A87AA62D4358}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>lp</t>
   </si>
@@ -50,190 +50,202 @@
     <t>Suma z błędów</t>
   </si>
   <si>
-    <t>Orlicka Maria</t>
-  </si>
-  <si>
-    <t>Tynna Beata</t>
-  </si>
-  <si>
-    <t>KAŹMIERCZAK SYLWIA</t>
-  </si>
-  <si>
-    <t>Rogozinska Katarzyna</t>
-  </si>
-  <si>
-    <t>Kraska Boguslawa</t>
-  </si>
-  <si>
-    <t>Zawierucha_ Ilona</t>
-  </si>
-  <si>
-    <t>SIMIŃSKA MAŁGORZATA</t>
-  </si>
-  <si>
-    <t>Czaplicka Anna</t>
-  </si>
-  <si>
-    <t>Urban Dorota</t>
-  </si>
-  <si>
-    <t>SZYNAL ELŻBIETA</t>
-  </si>
-  <si>
-    <t>SAS Aneta</t>
-  </si>
-  <si>
-    <t>SZYNAL ANNA</t>
-  </si>
-  <si>
-    <t>GÓRALCZYK ANNA</t>
-  </si>
-  <si>
-    <t>SIERPIEJKO KATARZYNA</t>
-  </si>
-  <si>
-    <t>HALMAN ANNA</t>
-  </si>
-  <si>
-    <t>Maksymiuk Andrzej</t>
-  </si>
-  <si>
-    <t>Gancarz Beata</t>
-  </si>
-  <si>
-    <t>Czajka Iwona</t>
-  </si>
-  <si>
-    <t>Jałowiecka Melania</t>
-  </si>
-  <si>
     <t>Rowicka Dorota</t>
   </si>
   <si>
-    <t>Szczepańska Małgorzata</t>
-  </si>
-  <si>
-    <t>LUKAS LUCYNA</t>
-  </si>
-  <si>
-    <t>Gil Anna</t>
-  </si>
-  <si>
-    <t>Gadek Agnieszka</t>
-  </si>
-  <si>
-    <t>KUZIO ADRIAN</t>
-  </si>
-  <si>
-    <t>Nowakowska Edyta</t>
-  </si>
-  <si>
-    <t>Żych Paulina</t>
-  </si>
-  <si>
-    <t>Skiba Aneta</t>
-  </si>
-  <si>
-    <t>Kasprzycka Renata</t>
-  </si>
-  <si>
     <t>Walczak Bartosz</t>
   </si>
   <si>
-    <t>Krawniak Zofia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JESCHKE KAROLINA </t>
-  </si>
-  <si>
-    <t>Bieniek Elżbieta</t>
-  </si>
-  <si>
-    <t>Giwojno Ilona</t>
-  </si>
-  <si>
-    <t>Matysiak Anna</t>
-  </si>
-  <si>
-    <t>Osowski Sebastian</t>
-  </si>
-  <si>
-    <t>Sobotot Adrian</t>
-  </si>
-  <si>
     <t>Tober Krzysztof</t>
   </si>
   <si>
-    <t>Michalak Jakub</t>
-  </si>
-  <si>
-    <t>MALLEK KAMIL</t>
-  </si>
-  <si>
-    <t>Stachnik_ Aleksandra</t>
-  </si>
-  <si>
-    <t>Antczak Dariusz</t>
-  </si>
-  <si>
-    <t>Swarcewicz_ Anna</t>
-  </si>
-  <si>
-    <t>Taudul Natalia</t>
-  </si>
-  <si>
-    <t>Pawulski Piotr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BUJNOWSKA VIOLETTA </t>
-  </si>
-  <si>
-    <t>Bulicki Zbigniew</t>
-  </si>
-  <si>
-    <t>Wójcicka Iwona</t>
-  </si>
-  <si>
     <t>Smołucha Aneta</t>
   </si>
   <si>
-    <t>Wojtkowska Anna</t>
-  </si>
-  <si>
-    <t>Hrybowicz Wojciech</t>
-  </si>
-  <si>
-    <t>PIOTROWSKI  GRZEGORZ</t>
-  </si>
-  <si>
-    <t>Siana Charisa</t>
-  </si>
-  <si>
-    <t>FIKRI MUHAMMAD RIZAL</t>
-  </si>
-  <si>
-    <t>Dura Salas</t>
-  </si>
-  <si>
-    <t>DOJOHARUDIN</t>
-  </si>
-  <si>
-    <t>Afrianto Heri</t>
-  </si>
-  <si>
-    <t>Nebab Ginia</t>
-  </si>
-  <si>
     <t>Maybenig Cendy</t>
   </si>
   <si>
-    <t>MENDEZ GALINDO ANNA MARIA</t>
-  </si>
-  <si>
-    <t>Botina Karen Tatiana</t>
-  </si>
-  <si>
-    <t>ORTEGA CARO JOEL DAVID</t>
+    <t>Tylutka Danuta</t>
+  </si>
+  <si>
+    <t>Szymborski Wojciech</t>
+  </si>
+  <si>
+    <t>Hajdasz Renata</t>
+  </si>
+  <si>
+    <t>Zadora Renata</t>
+  </si>
+  <si>
+    <t>Wróbel Katarzyna</t>
+  </si>
+  <si>
+    <t>Sikora Roman</t>
+  </si>
+  <si>
+    <t>Barszcz Paweł</t>
+  </si>
+  <si>
+    <t>Chmielewska Aneta</t>
+  </si>
+  <si>
+    <t>Kochan Anna</t>
+  </si>
+  <si>
+    <t>Bajdan Anna</t>
+  </si>
+  <si>
+    <t>Szulc Daria</t>
+  </si>
+  <si>
+    <t>Weryho Krzysztof</t>
+  </si>
+  <si>
+    <t>Hoptasz Wanda</t>
+  </si>
+  <si>
+    <t>Czajka Sara</t>
+  </si>
+  <si>
+    <t>Lutomska Karolina</t>
+  </si>
+  <si>
+    <t>Zulleidys Galvis</t>
+  </si>
+  <si>
+    <t>PINEDA PAEZ MARLON HESNEIDER</t>
+  </si>
+  <si>
+    <t>Diaz Guavita Johan Steven</t>
+  </si>
+  <si>
+    <t>BOGUSŁAWA KRASKA</t>
+  </si>
+  <si>
+    <t>AGNIESZKA HAŁUSZCZYK</t>
+  </si>
+  <si>
+    <t>Aneta SAS</t>
+  </si>
+  <si>
+    <t>MAREK JAROSZ</t>
+  </si>
+  <si>
+    <t>AGNIESZKA PIERWIENIECKA</t>
+  </si>
+  <si>
+    <t>ANDRZEJ MAKSYMIUK</t>
+  </si>
+  <si>
+    <t>ELŻBIETA CZAJKA</t>
+  </si>
+  <si>
+    <t>MELANIA JAŁOWIECKA</t>
+  </si>
+  <si>
+    <t>JOANNA PODOLSKA</t>
+  </si>
+  <si>
+    <t>AGNIESZKA NOWICKA</t>
+  </si>
+  <si>
+    <t>AGNIESZKA PANEK</t>
+  </si>
+  <si>
+    <t>KRYSTYNA ZAKRZEWSKA</t>
+  </si>
+  <si>
+    <t>EDYTA NOWAKOWSKA</t>
+  </si>
+  <si>
+    <t>KAMILA PAWULSKA</t>
+  </si>
+  <si>
+    <t>KAMIL CHWOJNICKI</t>
+  </si>
+  <si>
+    <t>MARIA ORLICKA</t>
+  </si>
+  <si>
+    <t>KRYSTYNA LIS-JODKO</t>
+  </si>
+  <si>
+    <t>ANETA SKIBA</t>
+  </si>
+  <si>
+    <t>ZOFIA KRAWNIAK</t>
+  </si>
+  <si>
+    <t>TOMASZ SZATKOWSKI</t>
+  </si>
+  <si>
+    <t>PATRYK JABŁOŃSKI</t>
+  </si>
+  <si>
+    <t>AGNIESZKA RESZTA</t>
+  </si>
+  <si>
+    <t>KRZYSZTOF WERYHO</t>
+  </si>
+  <si>
+    <t>DOMINIKA WADLEWSKA</t>
+  </si>
+  <si>
+    <t>KRZYSZTOF TOBER</t>
+  </si>
+  <si>
+    <t>ADRIAN JAŁOWIECKI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KRYSTNA  JAKOWICKA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANETA  SMOŁUCHA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEWERYN  PIETRZAK </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KARLIŃSKI MATEUSZ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOANNA  ZIEMIŃSKA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRZEGORZ PIOTROWSKI </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ALEKSANDRA  ABERBACH</t>
+  </si>
+  <si>
+    <t>Paulina Zawielak</t>
+  </si>
+  <si>
+    <t>Mariola Woźniak</t>
+  </si>
+  <si>
+    <t>Katarzyna Reszta</t>
+  </si>
+  <si>
+    <t>AGNIESZKA WILCHOWSKA</t>
+  </si>
+  <si>
+    <t>EWA GÓRALCZYK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LORNA  SORIANO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DILBER ANDREY  VILLADA BUITRAGO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOHAN STEVEN  DIAZ GUAVITA </t>
+  </si>
+  <si>
+    <t>ANDRZEJ ŚMICH</t>
+  </si>
+  <si>
+    <t>KATARZYNA ROGOZIŃSKA</t>
   </si>
 </sst>
 </file>
@@ -633,13 +645,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E83883C-EB99-482A-92BF-3645C56F7AE9}">
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A63"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62:A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -660,10 +677,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>21</v>
+        <v>173</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -674,10 +691,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>29</v>
+        <v>901</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
@@ -688,10 +705,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>76</v>
+        <v>905</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
@@ -702,10 +719,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>93</v>
+        <v>1673</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
@@ -716,10 +733,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>117</v>
+        <v>1734</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
@@ -730,13 +747,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>253</v>
+        <v>1798</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D7" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -744,10 +761,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>263</v>
+        <v>1877</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D8" s="2">
         <v>1</v>
@@ -758,10 +775,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>283</v>
+        <v>2132</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D9" s="2">
         <v>1</v>
@@ -772,10 +789,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>428</v>
+        <v>2189</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D10" s="2">
         <v>1</v>
@@ -786,10 +803,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>1354</v>
+        <v>2237</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D11" s="2">
         <v>1</v>
@@ -800,10 +817,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>1501</v>
+        <v>2286</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D12" s="2">
         <v>1</v>
@@ -814,10 +831,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="2">
-        <v>1515</v>
+        <v>2396</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D13" s="2">
         <v>1</v>
@@ -828,10 +845,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="2">
-        <v>1522</v>
+        <v>2532</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D14" s="2">
         <v>1</v>
@@ -842,13 +859,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="2">
-        <v>1702</v>
+        <v>2539</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D15" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -856,13 +873,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="2">
-        <v>1765</v>
+        <v>2624</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D16" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -870,10 +887,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="2">
-        <v>1789</v>
+        <v>2705</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="D17" s="2">
         <v>2</v>
@@ -884,10 +901,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="2">
-        <v>1799</v>
+        <v>2946</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D18" s="2">
         <v>1</v>
@@ -898,10 +915,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="2">
-        <v>1814</v>
+        <v>3165</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D19" s="2">
         <v>1</v>
@@ -912,13 +929,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="2">
-        <v>1825</v>
+        <v>3234</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D20" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -926,13 +943,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="2">
-        <v>1877</v>
+        <v>6102</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="D21" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -940,7 +957,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="2">
-        <v>1883</v>
+        <v>6130</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>24</v>
@@ -954,7 +971,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="2">
-        <v>1907</v>
+        <v>6166</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>25</v>
@@ -968,7 +985,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="2">
-        <v>1954</v>
+        <v>6187</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>26</v>
@@ -982,13 +999,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="2">
-        <v>1982</v>
+        <v>117</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D25" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -996,7 +1013,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="2">
-        <v>2009</v>
+        <v>1483</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>28</v>
@@ -1010,7 +1027,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="2">
-        <v>2022</v>
+        <v>1501</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>29</v>
@@ -1024,13 +1041,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="2">
-        <v>2037</v>
+        <v>1628</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D28" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1038,13 +1055,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="2">
-        <v>2104</v>
+        <v>1634</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D29" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1052,7 +1069,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="2">
-        <v>2118</v>
+        <v>1789</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>32</v>
@@ -1066,7 +1083,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="2">
-        <v>2132</v>
+        <v>1824</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>33</v>
@@ -1080,7 +1097,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="2">
-        <v>2136</v>
+        <v>1825</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>34</v>
@@ -1094,7 +1111,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="2">
-        <v>2139</v>
+        <v>1906</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>35</v>
@@ -1108,13 +1125,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="2">
-        <v>2150</v>
+        <v>1972</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D34" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1122,7 +1139,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="2">
-        <v>2262</v>
+        <v>1982</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>37</v>
@@ -1136,13 +1153,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="2">
-        <v>2293</v>
+        <v>1997</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>38</v>
       </c>
       <c r="D36" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1150,7 +1167,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="2">
-        <v>2612</v>
+        <v>2022</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>39</v>
@@ -1164,7 +1181,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="2">
-        <v>2697</v>
+        <v>2080</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>40</v>
@@ -1178,13 +1195,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="2">
-        <v>2705</v>
+        <v>2088</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D39" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1192,7 +1209,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="2">
-        <v>2706</v>
+        <v>21</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>42</v>
@@ -1206,7 +1223,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="2">
-        <v>2726</v>
+        <v>2101</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>43</v>
@@ -1220,13 +1237,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="2">
-        <v>2866</v>
+        <v>2104</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D42" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1234,7 +1251,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="2">
-        <v>2882</v>
+        <v>2136</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>45</v>
@@ -1248,7 +1265,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="2">
-        <v>2885</v>
+        <v>2192</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>46</v>
@@ -1262,7 +1279,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="2">
-        <v>2922</v>
+        <v>2218</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>47</v>
@@ -1276,7 +1293,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="2">
-        <v>2926</v>
+        <v>2518</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>48</v>
@@ -1290,7 +1307,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="2">
-        <v>2960</v>
+        <v>2539</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>49</v>
@@ -1304,7 +1321,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="2">
-        <v>3005</v>
+        <v>2598</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>50</v>
@@ -1318,13 +1335,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="2">
-        <v>3054</v>
+        <v>2705</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>51</v>
       </c>
       <c r="D49" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1332,7 +1349,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="2">
-        <v>3165</v>
+        <v>2812</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>52</v>
@@ -1346,13 +1363,13 @@
         <v>50</v>
       </c>
       <c r="B51" s="2">
-        <v>3179</v>
+        <v>3142</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>53</v>
       </c>
       <c r="D51" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1360,7 +1377,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="2">
-        <v>3185</v>
+        <v>3165</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>54</v>
@@ -1374,7 +1391,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="2">
-        <v>3243</v>
+        <v>3181</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>55</v>
@@ -1388,7 +1405,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="2">
-        <v>6009</v>
+        <v>3196</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>56</v>
@@ -1402,7 +1419,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="2">
-        <v>6025</v>
+        <v>3232</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>57</v>
@@ -1416,7 +1433,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="2">
-        <v>6034</v>
+        <v>3243</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>58</v>
@@ -1430,7 +1447,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="2">
-        <v>6058</v>
+        <v>3244</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>59</v>
@@ -1444,13 +1461,13 @@
         <v>57</v>
       </c>
       <c r="B58" s="2">
-        <v>6084</v>
+        <v>3249</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>60</v>
       </c>
       <c r="D58" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1458,7 +1475,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="2">
-        <v>6094</v>
+        <v>3254</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>61</v>
@@ -1472,7 +1489,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="2">
-        <v>6102</v>
+        <v>3255</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>62</v>
@@ -1486,13 +1503,13 @@
         <v>60</v>
       </c>
       <c r="B61" s="2">
-        <v>6105</v>
+        <v>357</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>63</v>
       </c>
       <c r="D61" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1500,7 +1517,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="2">
-        <v>6165</v>
+        <v>56</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>64</v>
@@ -1514,12 +1531,68 @@
         <v>62</v>
       </c>
       <c r="B63" s="2">
-        <v>6172</v>
+        <v>6176</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>65</v>
       </c>
       <c r="D63" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64">
+        <v>6186</v>
+      </c>
+      <c r="C64" t="s">
+        <v>66</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <v>6187</v>
+      </c>
+      <c r="C65" t="s">
+        <v>67</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66">
+        <v>69</v>
+      </c>
+      <c r="C66" t="s">
+        <v>68</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67">
+        <v>93</v>
+      </c>
+      <c r="C67" t="s">
+        <v>69</v>
+      </c>
+      <c r="D67">
         <v>1</v>
       </c>
     </row>

</xml_diff>